<commit_message>
TitanicNormalised and some version changes
</commit_message>
<xml_diff>
--- a/results/titanicNumeric/35/chars_of_network.xlsx
+++ b/results/titanicNumeric/35/chars_of_network.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>CHARACTERISTICS OF THE TRAINED NETWORK</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Average standard deviation from center:</t>
   </si>
   <si>
-    <t>0.32408953865815704</t>
+    <t>0.26607752571579923</t>
   </si>
   <si>
     <t>Porcentage zero weights:</t>
@@ -55,25 +55,19 @@
     <t>Train</t>
   </si>
   <si>
-    <t>0.382262996941896</t>
-  </si>
-  <si>
-    <t>0.36904761904761907</t>
-  </si>
-  <si>
-    <t>0.868</t>
+    <t>0.617737003058104</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>0.3801526717557252</t>
-  </si>
-  <si>
-    <t>0.3704318936877076</t>
-  </si>
-  <si>
-    <t>0.892</t>
+    <t>0.6183206106870229</t>
   </si>
 </sst>
 </file>
@@ -480,7 +474,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -491,7 +485,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>